<commit_message>
checking in the fixes for the tests which were failing. for all 8 tests
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Add_GF_Protein.xlsx
+++ b/src/main/resources/testdata/Add_GF_Protein.xlsx
@@ -69,9 +69,6 @@
     <t>TaEXPB23</t>
   </si>
   <si>
-    <t>AY260547.prot</t>
-  </si>
-  <si>
     <t>Avena sativa</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>SeleniumProtein</t>
+  </si>
+  <si>
+    <t>angaj2010</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,13 +489,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -537,7 +537,7 @@
         <v>14</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -545,55 +545,55 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing the new tests and changes in the tests.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Add_GF_Protein.xlsx
+++ b/src/main/resources/testdata/Add_GF_Protein.xlsx
@@ -63,9 +63,6 @@
     <t>accessionNoGS</t>
   </si>
   <si>
-    <t>1 marvsanava lvalvsvllt ygccaqspln ytgslakssk aswswlpaka twygaptgag 61 pddnggacgy khtnqypfms mtscgneplf kdgmgcgacy qircvnnkac sgkpetvmit 121 dmnyypvgky hfdlsgtafg amakpgqndk lrhagiidiq  fqrvpcnhpg lnvnfqverg 181 snpnylavlv efanregtvv qmdlmesrng rptgywtamr hswgaiwrmd srrrlqgpfs 241 lrirsesgkt lvakqvipan wrpdtnyrsn vqfr</t>
-  </si>
-  <si>
     <t>TaEXPB23</t>
   </si>
   <si>
@@ -114,7 +111,11 @@
     <t>SeleniumProtein</t>
   </si>
   <si>
-    <t>angaj2010</t>
+    <t xml:space="preserve">
+1 marvsanava lvalvsvllt ygccaqspln ytgslakssk aswswlpaka twygaptgag 61 pddnggacgy khtnqypfms mtscgneplf kdgmgcgacy qircvnnkac sgkpetvmit 121 dmnyypvgky hfdlsgtafg amakpgqndk lrhagiidiq  fqrvpcnhpg lnvnfqverg 181 snpnylavlv efanregtvv qmdlmesrng rptgywtamr hswgaiwrmd srrrlqgpfs 241 lrirsesgkt lvakqvipan wrpdtnyrsn vqfr</t>
+  </si>
+  <si>
+    <t>Protein_selenium</t>
   </si>
 </sst>
 </file>
@@ -458,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,20 +469,21 @@
     <col min="2" max="2" width="29.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="17" max="17" width="18" style="1" customWidth="1"/>
+    <col min="18" max="18" width="25.42578125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -489,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -537,63 +539,63 @@
         <v>14</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing the changes (maintenance ) in failing tests.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Add_GF_Protein.xlsx
+++ b/src/main/resources/testdata/Add_GF_Protein.xlsx
@@ -115,7 +115,7 @@
 1 marvsanava lvalvsvllt ygccaqspln ytgslakssk aswswlpaka twygaptgag 61 pddnggacgy khtnqypfms mtscgneplf kdgmgcgacy qircvnnkac sgkpetvmit 121 dmnyypvgky hfdlsgtafg amakpgqndk lrhagiidiq  fqrvpcnhpg lnvnfqverg 181 snpnylavlv efanregtvv qmdlmesrng rptgywtamr hswgaiwrmd srrrlqgpfs 241 lrirsesgkt lvakqvipan wrpdtnyrsn vqfr</t>
   </si>
   <si>
-    <t>Protein_selenium</t>
+    <t>SYLK003883-PROT.prot</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,10 +483,11 @@
     <col min="16" max="16" width="9.140625" style="1"/>
     <col min="17" max="17" width="18" style="1" customWidth="1"/>
     <col min="18" max="18" width="25.42578125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="19" max="19" width="17.85546875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>